<commit_message>
No more concstant scraping, exchanging Dollar stocks to EUR before PF line
</commit_message>
<xml_diff>
--- a/investing_source_example.xlsx
+++ b/investing_source_example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Robin/Documents/personal_finance/Investing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Robin/Documents/personal_finance/Investing/Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BACBA5D-F364-B046-BE31-A944241FF2AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8A7E03-0B52-4642-9C21-166048B83A67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17540" xr2:uid="{9686E4FC-88CA-2049-8D43-579C3AB447BB}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Budget" sheetId="2" r:id="rId2"/>
     <sheet name="Interests" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -474,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51C62995-213B-F64C-869F-3A78F5C97F52}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -588,10 +588,45 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>44062</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>440</v>
+      </c>
+      <c r="F4">
+        <v>372.52</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>0.5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -628,7 +663,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A6" sqref="A6:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -760,39 +795,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>44144</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>440</v>
-      </c>
-      <c r="F9">
-        <v>400</v>
-      </c>
-      <c r="G9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9">
-        <v>0.5</v>
-      </c>
-      <c r="I9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" t="s">
-        <v>21</v>
-      </c>
+      <c r="A9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>